<commit_message>
added graphics and monthly conditioned loads table
</commit_message>
<xml_diff>
--- a/input/BSIMAC/9.9.0.7.4/RESULTS5-2A.xlsx
+++ b/input/BSIMAC/9.9.0.7.4/RESULTS5-2A.xlsx
@@ -2037,7 +2037,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
@@ -2045,7 +2045,7 @@
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
@@ -2332,13 +2332,13 @@
   </sheetPr>
   <dimension ref="A3:AO579"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A118" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C130" activeCellId="0" sqref="C130"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A180" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C191" activeCellId="0" sqref="C191"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="8" style="0" width="10.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="18" style="0" width="9.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="26" style="0" width="10.53"/>
@@ -5198,253 +5198,625 @@
       <c r="B190" s="120" t="s">
         <v>13</v>
       </c>
-      <c r="C190" s="59"/>
-      <c r="D190" s="121"/>
-      <c r="E190" s="57"/>
-      <c r="F190" s="56"/>
-      <c r="G190" s="61"/>
-      <c r="H190" s="56"/>
-      <c r="I190" s="56"/>
-      <c r="J190" s="56"/>
-      <c r="K190" s="59"/>
-      <c r="L190" s="121"/>
-      <c r="M190" s="56"/>
-      <c r="N190" s="56"/>
-      <c r="O190" s="56"/>
-      <c r="P190" s="57"/>
-      <c r="Q190" s="56"/>
-      <c r="R190" s="62"/>
+      <c r="C190" s="59" t="n">
+        <v>664</v>
+      </c>
+      <c r="D190" s="121" t="n">
+        <v>475.4</v>
+      </c>
+      <c r="E190" s="57" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="F190" s="56" t="n">
+        <v>29</v>
+      </c>
+      <c r="G190" s="61" t="n">
+        <v>7</v>
+      </c>
+      <c r="H190" s="56" t="n">
+        <v>5.65</v>
+      </c>
+      <c r="I190" s="56" t="n">
+        <v>22</v>
+      </c>
+      <c r="J190" s="56" t="n">
+        <v>15</v>
+      </c>
+      <c r="K190" s="59" t="n">
+        <v>277.8</v>
+      </c>
+      <c r="L190" s="121" t="n">
+        <v>73.3</v>
+      </c>
+      <c r="M190" s="56" t="n">
+        <v>2.322</v>
+      </c>
+      <c r="N190" s="56" t="n">
+        <v>7</v>
+      </c>
+      <c r="O190" s="56" t="n">
+        <v>7</v>
+      </c>
+      <c r="P190" s="57" t="n">
+        <v>1.982</v>
+      </c>
+      <c r="Q190" s="56" t="n">
+        <v>22</v>
+      </c>
+      <c r="R190" s="62" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B191" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="C191" s="59"/>
-      <c r="D191" s="121"/>
-      <c r="E191" s="57"/>
-      <c r="F191" s="56"/>
-      <c r="G191" s="61"/>
-      <c r="H191" s="56"/>
-      <c r="I191" s="56"/>
-      <c r="J191" s="56"/>
-      <c r="K191" s="59"/>
-      <c r="L191" s="121"/>
-      <c r="M191" s="56"/>
-      <c r="N191" s="56"/>
-      <c r="O191" s="56"/>
-      <c r="P191" s="57"/>
-      <c r="Q191" s="56"/>
-      <c r="R191" s="62"/>
+      <c r="C191" s="59" t="n">
+        <v>653.3</v>
+      </c>
+      <c r="D191" s="121" t="n">
+        <v>349.2</v>
+      </c>
+      <c r="E191" s="57" t="n">
+        <v>3.041</v>
+      </c>
+      <c r="F191" s="56" t="n">
+        <v>9</v>
+      </c>
+      <c r="G191" s="61" t="n">
+        <v>7</v>
+      </c>
+      <c r="H191" s="56" t="n">
+        <v>4.921</v>
+      </c>
+      <c r="I191" s="56" t="n">
+        <v>15</v>
+      </c>
+      <c r="J191" s="56" t="n">
+        <v>15</v>
+      </c>
+      <c r="K191" s="59" t="n">
+        <v>307.4</v>
+      </c>
+      <c r="L191" s="121" t="n">
+        <v>24</v>
+      </c>
+      <c r="M191" s="56" t="n">
+        <v>2.551</v>
+      </c>
+      <c r="N191" s="56" t="n">
+        <v>8</v>
+      </c>
+      <c r="O191" s="56" t="n">
+        <v>24</v>
+      </c>
+      <c r="P191" s="57" t="n">
+        <v>1.096</v>
+      </c>
+      <c r="Q191" s="56" t="n">
+        <v>15</v>
+      </c>
+      <c r="R191" s="62" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B192" s="120" t="s">
         <v>17</v>
       </c>
-      <c r="C192" s="59"/>
-      <c r="D192" s="121"/>
-      <c r="E192" s="57"/>
-      <c r="F192" s="56"/>
-      <c r="G192" s="61"/>
-      <c r="H192" s="56"/>
-      <c r="I192" s="56"/>
-      <c r="J192" s="56"/>
-      <c r="K192" s="59"/>
-      <c r="L192" s="121"/>
-      <c r="M192" s="56"/>
-      <c r="N192" s="56"/>
-      <c r="O192" s="56"/>
-      <c r="P192" s="57"/>
-      <c r="Q192" s="56"/>
-      <c r="R192" s="62"/>
+      <c r="C192" s="59" t="n">
+        <v>433.5</v>
+      </c>
+      <c r="D192" s="121" t="n">
+        <v>450.3</v>
+      </c>
+      <c r="E192" s="57" t="n">
+        <v>2.275</v>
+      </c>
+      <c r="F192" s="56" t="n">
+        <v>2</v>
+      </c>
+      <c r="G192" s="61" t="n">
+        <v>7</v>
+      </c>
+      <c r="H192" s="56" t="n">
+        <v>4.458</v>
+      </c>
+      <c r="I192" s="56" t="n">
+        <v>24</v>
+      </c>
+      <c r="J192" s="56" t="n">
+        <v>14</v>
+      </c>
+      <c r="K192" s="59" t="n">
+        <v>134.4</v>
+      </c>
+      <c r="L192" s="121" t="n">
+        <v>86.4</v>
+      </c>
+      <c r="M192" s="56" t="n">
+        <v>1.774</v>
+      </c>
+      <c r="N192" s="56" t="n">
+        <v>16</v>
+      </c>
+      <c r="O192" s="56" t="n">
+        <v>7</v>
+      </c>
+      <c r="P192" s="57" t="n">
+        <v>1.508</v>
+      </c>
+      <c r="Q192" s="56" t="n">
+        <v>10</v>
+      </c>
+      <c r="R192" s="62" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B193" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="C193" s="59"/>
-      <c r="D193" s="121"/>
-      <c r="E193" s="57"/>
-      <c r="F193" s="56"/>
-      <c r="G193" s="61"/>
-      <c r="H193" s="56"/>
-      <c r="I193" s="56"/>
-      <c r="J193" s="56"/>
-      <c r="K193" s="59"/>
-      <c r="L193" s="121"/>
-      <c r="M193" s="56"/>
-      <c r="N193" s="56"/>
-      <c r="O193" s="56"/>
-      <c r="P193" s="57"/>
-      <c r="Q193" s="56"/>
-      <c r="R193" s="62"/>
+      <c r="C193" s="59" t="n">
+        <v>511</v>
+      </c>
+      <c r="D193" s="121" t="n">
+        <v>218.7</v>
+      </c>
+      <c r="E193" s="57" t="n">
+        <v>2.446</v>
+      </c>
+      <c r="F193" s="56" t="n">
+        <v>3</v>
+      </c>
+      <c r="G193" s="61" t="n">
+        <v>6</v>
+      </c>
+      <c r="H193" s="56" t="n">
+        <v>3.473</v>
+      </c>
+      <c r="I193" s="56" t="n">
+        <v>12</v>
+      </c>
+      <c r="J193" s="56" t="n">
+        <v>14</v>
+      </c>
+      <c r="K193" s="59" t="n">
+        <v>275.7</v>
+      </c>
+      <c r="L193" s="121" t="n">
+        <v>29.3</v>
+      </c>
+      <c r="M193" s="56" t="n">
+        <v>1.997</v>
+      </c>
+      <c r="N193" s="56" t="n">
+        <v>2</v>
+      </c>
+      <c r="O193" s="56" t="n">
+        <v>7</v>
+      </c>
+      <c r="P193" s="57" t="n">
+        <v>1.093</v>
+      </c>
+      <c r="Q193" s="56" t="n">
+        <v>7</v>
+      </c>
+      <c r="R193" s="62" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B194" s="120" t="s">
         <v>21</v>
       </c>
-      <c r="C194" s="59"/>
-      <c r="D194" s="121"/>
-      <c r="E194" s="57"/>
-      <c r="F194" s="56"/>
-      <c r="G194" s="61"/>
-      <c r="H194" s="56"/>
-      <c r="I194" s="56"/>
-      <c r="J194" s="56"/>
-      <c r="K194" s="59"/>
-      <c r="L194" s="121"/>
-      <c r="M194" s="56"/>
-      <c r="N194" s="56"/>
-      <c r="O194" s="56"/>
-      <c r="P194" s="57"/>
-      <c r="Q194" s="56"/>
-      <c r="R194" s="62"/>
+      <c r="C194" s="59" t="n">
+        <v>112.8</v>
+      </c>
+      <c r="D194" s="121" t="n">
+        <v>342.7</v>
+      </c>
+      <c r="E194" s="57" t="n">
+        <v>1.645</v>
+      </c>
+      <c r="F194" s="56" t="n">
+        <v>3</v>
+      </c>
+      <c r="G194" s="61" t="n">
+        <v>5</v>
+      </c>
+      <c r="H194" s="56" t="n">
+        <v>2.774</v>
+      </c>
+      <c r="I194" s="56" t="n">
+        <v>10</v>
+      </c>
+      <c r="J194" s="56" t="n">
+        <v>14</v>
+      </c>
+      <c r="K194" s="59" t="n">
+        <v>20.1</v>
+      </c>
+      <c r="L194" s="121" t="n">
+        <v>131.1</v>
+      </c>
+      <c r="M194" s="56" t="n">
+        <v>1.295</v>
+      </c>
+      <c r="N194" s="56" t="n">
+        <v>4</v>
+      </c>
+      <c r="O194" s="56" t="n">
+        <v>6</v>
+      </c>
+      <c r="P194" s="57" t="n">
+        <v>1.555</v>
+      </c>
+      <c r="Q194" s="56" t="n">
+        <v>11</v>
+      </c>
+      <c r="R194" s="62" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B195" s="120" t="s">
         <v>23</v>
       </c>
-      <c r="C195" s="59"/>
-      <c r="D195" s="121"/>
-      <c r="E195" s="57"/>
-      <c r="F195" s="56"/>
-      <c r="G195" s="61"/>
-      <c r="H195" s="56"/>
-      <c r="I195" s="56"/>
-      <c r="J195" s="56"/>
-      <c r="K195" s="59"/>
-      <c r="L195" s="121"/>
-      <c r="M195" s="56"/>
+      <c r="C195" s="59" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D195" s="121" t="n">
+        <v>578.3</v>
+      </c>
+      <c r="E195" s="57" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="F195" s="56" t="n">
+        <v>9</v>
+      </c>
+      <c r="G195" s="61" t="n">
+        <v>5</v>
+      </c>
+      <c r="H195" s="56" t="n">
+        <v>3.253</v>
+      </c>
+      <c r="I195" s="56" t="n">
+        <v>26</v>
+      </c>
+      <c r="J195" s="56" t="n">
+        <v>15</v>
+      </c>
+      <c r="K195" s="59" t="n">
+        <v>0</v>
+      </c>
+      <c r="L195" s="121" t="n">
+        <v>447.5</v>
+      </c>
+      <c r="M195" s="56" t="n">
+        <v>0</v>
+      </c>
       <c r="N195" s="56"/>
       <c r="O195" s="56"/>
-      <c r="P195" s="57"/>
-      <c r="Q195" s="56"/>
-      <c r="R195" s="62"/>
+      <c r="P195" s="57" t="n">
+        <v>2.101</v>
+      </c>
+      <c r="Q195" s="56" t="n">
+        <v>26</v>
+      </c>
+      <c r="R195" s="62" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B196" s="120" t="s">
         <v>25</v>
       </c>
-      <c r="C196" s="59"/>
-      <c r="D196" s="121"/>
-      <c r="E196" s="57"/>
-      <c r="F196" s="56"/>
-      <c r="G196" s="61"/>
-      <c r="H196" s="56"/>
-      <c r="I196" s="56"/>
-      <c r="J196" s="56"/>
-      <c r="K196" s="59"/>
-      <c r="L196" s="121"/>
-      <c r="M196" s="56"/>
+      <c r="C196" s="59" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="D196" s="121" t="n">
+        <v>568.4</v>
+      </c>
+      <c r="E196" s="57" t="n">
+        <v>0.599</v>
+      </c>
+      <c r="F196" s="56" t="n">
+        <v>25</v>
+      </c>
+      <c r="G196" s="61" t="n">
+        <v>6</v>
+      </c>
+      <c r="H196" s="56" t="n">
+        <v>3.319</v>
+      </c>
+      <c r="I196" s="56" t="n">
+        <v>17</v>
+      </c>
+      <c r="J196" s="56" t="n">
+        <v>14</v>
+      </c>
+      <c r="K196" s="59" t="n">
+        <v>0</v>
+      </c>
+      <c r="L196" s="121" t="n">
+        <v>440.9</v>
+      </c>
+      <c r="M196" s="56" t="n">
+        <v>0</v>
+      </c>
       <c r="N196" s="56"/>
       <c r="O196" s="56"/>
-      <c r="P196" s="57"/>
-      <c r="Q196" s="56"/>
-      <c r="R196" s="62"/>
+      <c r="P196" s="57" t="n">
+        <v>2.14</v>
+      </c>
+      <c r="Q196" s="56" t="n">
+        <v>17</v>
+      </c>
+      <c r="R196" s="62" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B197" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="C197" s="59"/>
-      <c r="D197" s="121"/>
-      <c r="E197" s="57"/>
-      <c r="F197" s="56"/>
-      <c r="G197" s="61"/>
-      <c r="H197" s="56"/>
-      <c r="I197" s="56"/>
-      <c r="J197" s="56"/>
-      <c r="K197" s="59"/>
-      <c r="L197" s="121"/>
-      <c r="M197" s="56"/>
+      <c r="C197" s="59" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="D197" s="121" t="n">
+        <v>658.2</v>
+      </c>
+      <c r="E197" s="57" t="n">
+        <v>0.572</v>
+      </c>
+      <c r="F197" s="56" t="n">
+        <v>10</v>
+      </c>
+      <c r="G197" s="61" t="n">
+        <v>7</v>
+      </c>
+      <c r="H197" s="56" t="n">
+        <v>4.192</v>
+      </c>
+      <c r="I197" s="56" t="n">
+        <v>26</v>
+      </c>
+      <c r="J197" s="56" t="n">
+        <v>14</v>
+      </c>
+      <c r="K197" s="59" t="n">
+        <v>0</v>
+      </c>
+      <c r="L197" s="121" t="n">
+        <v>532.6</v>
+      </c>
+      <c r="M197" s="56" t="n">
+        <v>0</v>
+      </c>
       <c r="N197" s="56"/>
       <c r="O197" s="56"/>
-      <c r="P197" s="57"/>
-      <c r="Q197" s="56"/>
-      <c r="R197" s="62"/>
+      <c r="P197" s="57" t="n">
+        <v>2.632</v>
+      </c>
+      <c r="Q197" s="56" t="n">
+        <v>26</v>
+      </c>
+      <c r="R197" s="62" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B198" s="120" t="s">
         <v>29</v>
       </c>
-      <c r="C198" s="59"/>
-      <c r="D198" s="121"/>
-      <c r="E198" s="57"/>
-      <c r="F198" s="56"/>
-      <c r="G198" s="61"/>
-      <c r="H198" s="56"/>
-      <c r="I198" s="56"/>
-      <c r="J198" s="56"/>
-      <c r="K198" s="59"/>
-      <c r="L198" s="121"/>
-      <c r="M198" s="56"/>
-      <c r="N198" s="56"/>
-      <c r="O198" s="56"/>
-      <c r="P198" s="57"/>
-      <c r="Q198" s="56"/>
-      <c r="R198" s="62"/>
+      <c r="C198" s="59" t="n">
+        <v>51.8</v>
+      </c>
+      <c r="D198" s="121" t="n">
+        <v>724.8</v>
+      </c>
+      <c r="E198" s="57" t="n">
+        <v>1.229</v>
+      </c>
+      <c r="F198" s="56" t="n">
+        <v>28</v>
+      </c>
+      <c r="G198" s="61" t="n">
+        <v>24</v>
+      </c>
+      <c r="H198" s="56" t="n">
+        <v>5.086</v>
+      </c>
+      <c r="I198" s="56" t="n">
+        <v>30</v>
+      </c>
+      <c r="J198" s="56" t="n">
+        <v>14</v>
+      </c>
+      <c r="K198" s="59" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="L198" s="121" t="n">
+        <v>517.9</v>
+      </c>
+      <c r="M198" s="56" t="n">
+        <v>0.113</v>
+      </c>
+      <c r="N198" s="56" t="n">
+        <v>28</v>
+      </c>
+      <c r="O198" s="56" t="n">
+        <v>6</v>
+      </c>
+      <c r="P198" s="57" t="n">
+        <v>2.961</v>
+      </c>
+      <c r="Q198" s="56" t="n">
+        <v>30</v>
+      </c>
+      <c r="R198" s="62" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B199" s="120" t="s">
         <v>31</v>
       </c>
-      <c r="C199" s="59"/>
-      <c r="D199" s="121"/>
-      <c r="E199" s="57"/>
-      <c r="F199" s="56"/>
-      <c r="G199" s="61"/>
-      <c r="H199" s="56"/>
-      <c r="I199" s="56"/>
-      <c r="J199" s="56"/>
-      <c r="K199" s="59"/>
-      <c r="L199" s="121"/>
-      <c r="M199" s="56"/>
-      <c r="N199" s="56"/>
-      <c r="O199" s="56"/>
-      <c r="P199" s="57"/>
-      <c r="Q199" s="56"/>
-      <c r="R199" s="62"/>
+      <c r="C199" s="59" t="n">
+        <v>317</v>
+      </c>
+      <c r="D199" s="121" t="n">
+        <v>628.4</v>
+      </c>
+      <c r="E199" s="57" t="n">
+        <v>1.702</v>
+      </c>
+      <c r="F199" s="56" t="n">
+        <v>6</v>
+      </c>
+      <c r="G199" s="61" t="n">
+        <v>7</v>
+      </c>
+      <c r="H199" s="56" t="n">
+        <v>5.577</v>
+      </c>
+      <c r="I199" s="56" t="n">
+        <v>18</v>
+      </c>
+      <c r="J199" s="56" t="n">
+        <v>14</v>
+      </c>
+      <c r="K199" s="59" t="n">
+        <v>80.5</v>
+      </c>
+      <c r="L199" s="121" t="n">
+        <v>296.2</v>
+      </c>
+      <c r="M199" s="56" t="n">
+        <v>1.201</v>
+      </c>
+      <c r="N199" s="56" t="n">
+        <v>6</v>
+      </c>
+      <c r="O199" s="56" t="n">
+        <v>7</v>
+      </c>
+      <c r="P199" s="57" t="n">
+        <v>3.039</v>
+      </c>
+      <c r="Q199" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="R199" s="62" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B200" s="120" t="s">
         <v>33</v>
       </c>
-      <c r="C200" s="59"/>
-      <c r="D200" s="121"/>
-      <c r="E200" s="57"/>
-      <c r="F200" s="56"/>
-      <c r="G200" s="61"/>
-      <c r="H200" s="56"/>
-      <c r="I200" s="56"/>
-      <c r="J200" s="56"/>
-      <c r="K200" s="59"/>
-      <c r="L200" s="121"/>
-      <c r="M200" s="56"/>
-      <c r="N200" s="56"/>
-      <c r="O200" s="56"/>
-      <c r="P200" s="57"/>
-      <c r="Q200" s="56"/>
-      <c r="R200" s="62"/>
+      <c r="C200" s="59" t="n">
+        <v>598.7</v>
+      </c>
+      <c r="D200" s="121" t="n">
+        <v>394.3</v>
+      </c>
+      <c r="E200" s="57" t="n">
+        <v>3.255</v>
+      </c>
+      <c r="F200" s="56" t="n">
+        <v>26</v>
+      </c>
+      <c r="G200" s="61" t="n">
+        <v>8</v>
+      </c>
+      <c r="H200" s="56" t="n">
+        <v>5.476</v>
+      </c>
+      <c r="I200" s="56" t="n">
+        <v>28</v>
+      </c>
+      <c r="J200" s="56" t="n">
+        <v>14</v>
+      </c>
+      <c r="K200" s="59" t="n">
+        <v>298.2</v>
+      </c>
+      <c r="L200" s="121" t="n">
+        <v>72.7</v>
+      </c>
+      <c r="M200" s="56" t="n">
+        <v>2.427</v>
+      </c>
+      <c r="N200" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="O200" s="56" t="n">
+        <v>7</v>
+      </c>
+      <c r="P200" s="57" t="n">
+        <v>1.982</v>
+      </c>
+      <c r="Q200" s="56" t="n">
+        <v>6</v>
+      </c>
+      <c r="R200" s="62" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B201" s="122" t="s">
         <v>35</v>
       </c>
-      <c r="C201" s="66"/>
-      <c r="D201" s="123"/>
-      <c r="E201" s="86"/>
-      <c r="F201" s="68"/>
-      <c r="G201" s="69"/>
-      <c r="H201" s="68"/>
-      <c r="I201" s="68"/>
-      <c r="J201" s="68"/>
-      <c r="K201" s="66"/>
-      <c r="L201" s="123"/>
-      <c r="M201" s="68"/>
-      <c r="N201" s="68"/>
-      <c r="O201" s="68"/>
-      <c r="P201" s="86"/>
-      <c r="Q201" s="68"/>
-      <c r="R201" s="70"/>
+      <c r="C201" s="66" t="n">
+        <v>698.7</v>
+      </c>
+      <c r="D201" s="123" t="n">
+        <v>433.3</v>
+      </c>
+      <c r="E201" s="86" t="n">
+        <v>3.171</v>
+      </c>
+      <c r="F201" s="68" t="n">
+        <v>31</v>
+      </c>
+      <c r="G201" s="69" t="n">
+        <v>24</v>
+      </c>
+      <c r="H201" s="68" t="n">
+        <v>5.537</v>
+      </c>
+      <c r="I201" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="J201" s="68" t="n">
+        <v>14</v>
+      </c>
+      <c r="K201" s="66" t="n">
+        <v>329.8</v>
+      </c>
+      <c r="L201" s="123" t="n">
+        <v>62.1</v>
+      </c>
+      <c r="M201" s="68" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="N201" s="68" t="n">
+        <v>31</v>
+      </c>
+      <c r="O201" s="68" t="n">
+        <v>8</v>
+      </c>
+      <c r="P201" s="86" t="n">
+        <v>2.069</v>
+      </c>
+      <c r="Q201" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="R201" s="70" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O202" s="124"/>

</xml_diff>